<commit_message>
update several column header descriptions
Some entries in the template aimed at curators are not suitable to appear in the Dashboard itself, e.g. as vaccine VO codes get converted to vaccine names.
</commit_message>
<xml_diff>
--- a/reformatted_data/gene_expression-recreated_template.xlsx
+++ b/reformatted_data/gene_expression-recreated_template.xlsx
@@ -1481,7 +1481,7 @@
     <t>observed</t>
   </si>
   <si>
-    <t>Any characteristics of the population(s) studied, plus whether the result was taken from a subgroup of the cohort tested.</t>
+    <t>Cohort - any characteristics of the population(s) studied, plus whether the result was taken from a subgroup of the broader cohort tested.</t>
   </si>
   <si>
     <t>Caucasian males, subgroup high responders</t>
@@ -3245,7 +3245,7 @@
     <t>vaccine</t>
   </si>
   <si>
-    <t>exposure material vaccine ontology ID (VO)</t>
+    <t>exposure material</t>
   </si>
   <si>
     <t>VO:0000045; VO:0000046</t>
@@ -3413,7 +3413,7 @@
     <t>VO:0000642</t>
   </si>
   <si>
-    <t>exposure material - additional</t>
+    <t>additional exposure material</t>
   </si>
   <si>
     <t>Live attenuated vaccine TC-83 challenge</t>
@@ -4847,7 +4847,7 @@
     <t>Top functional network for genes preferentially upregulated in the high responder group</t>
   </si>
   <si>
-    <t>only TIFA was significantly differentially expressed at the concerned time point compared with baseline (D0 log2 mean expression, 3.38; D1 log2 fold change, 1.33; multiplicity-adjusted p value, 1.14E-09; Figure S6)</t>
+    <t>Only TIFA was significantly differentially expressed at the concerned time point compared with baseline (D0 log2 mean expression, 3.38; D1 log2 fold change, 1.33; multiplicity-adjusted p value, 1.14E-09; Figure S6)</t>
   </si>
   <si>
     <t>Genes in BTM M75</t>
@@ -5627,10 +5627,10 @@
     <t>347</t>
   </si>
   <si>
-    <t>ID of observation within its own submission</t>
-  </si>
-  <si>
-    <t>Uniq ID of observation within its submission type</t>
+    <t xml:space="preserve">ID of observation within a publication (PMID) and for its submission type </t>
+  </si>
+  <si>
+    <t>ID of observation within its submission type</t>
   </si>
   <si>
     <t>59</t>

</xml_diff>